<commit_message>
Updating test to handle the class format
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>-2000000</v>
+        <v>-1000000</v>
       </c>
     </row>
     <row r="3">
@@ -534,34 +534,34 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>60000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4">
@@ -571,34 +571,34 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>1050000</v>
+        <v>489999.9999999999</v>
       </c>
     </row>
     <row r="5">
@@ -611,34 +611,34 @@
         <v>-140000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
     </row>
     <row r="6">
@@ -658,10 +658,10 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>-100000</v>
+        <v>-300000</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>100000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="8">
@@ -671,37 +671,37 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-2240000</v>
+        <v>-1440000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="H8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>760000</v>
+        <v>379999.9999999999</v>
       </c>
       <c r="L8" s="9" t="n">
-        <v>1000000</v>
+        <v>820000</v>
       </c>
     </row>
     <row r="9">
@@ -711,37 +711,37 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-2240000</v>
+        <v>-1440000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>687782.8054298642</v>
+        <v>343891.4027149321</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>622427.8782170718</v>
+        <v>311213.9391085358</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>563283.1477077572</v>
+        <v>281641.5738538786</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>509758.5047129025</v>
+        <v>254879.2523564512</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>461319.9137673326</v>
+        <v>230659.9568836663</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>417484.0848573145</v>
+        <v>208742.0424286572</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>377813.6514545833</v>
+        <v>188906.8257272916</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>341912.8067462292</v>
+        <v>170956.4033731146</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>309423.3545214745</v>
+        <v>154711.6772607372</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>368448.8622546731</v>
+        <v>302128.0670488319</v>
       </c>
     </row>
     <row r="10">
@@ -751,37 +751,37 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-2240000</v>
+        <v>-1440000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-1552217.194570136</v>
+        <v>-1096108.597285068</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>-929789.316353064</v>
+        <v>-784894.658176532</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>-366506.1686453068</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <v>143252.3360675956</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <v>604572.2498349282</v>
+        <v>-503253.0843226534</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>-248373.8319662022</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>-17713.87508253596</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>1022056.334692243</v>
+        <v>191028.1673461213</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>1399869.986146826</v>
+        <v>379934.9930734129</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>1741782.792893055</v>
+        <v>550891.3964465274</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>2051206.14741453</v>
+        <v>705603.0737072646</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>2419655.009669203</v>
+        <v>1007731.140756096</v>
       </c>
     </row>
     <row r="11">
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>2419655.009669203</v>
+        <v>1007731.140756096</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Username and password attributes added and integrated
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>-1500000</v>
+        <v>-1000000</v>
       </c>
     </row>
     <row r="3">
@@ -534,34 +534,34 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>45000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4">
@@ -571,34 +571,34 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
     </row>
     <row r="5">
@@ -608,37 +608,37 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-210000</v>
+        <v>-350000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>-350000</v>
+        <v>-700000</v>
       </c>
     </row>
     <row r="6">
@@ -671,37 +671,37 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-1910000</v>
+        <v>-1550000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="H8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>395000</v>
+        <v>730000</v>
       </c>
       <c r="L8" s="9" t="n">
-        <v>735000</v>
+        <v>1070000</v>
       </c>
     </row>
     <row r="9">
@@ -711,37 +711,37 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-1910000</v>
+        <v>-1550000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>364391.1439114391</v>
+        <v>673431.7343173431</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>336154.1918002206</v>
+        <v>621246.9873776227</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>310105.3429891333</v>
+        <v>573106.0769166261</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>286075.0396578721</v>
+        <v>528695.6429120167</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>263906.8631530185</v>
+        <v>487726.6078524138</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>243456.5158238178</v>
+        <v>449932.2950668024</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>224590.8817562894</v>
+        <v>415066.6928660539</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>207187.1602917799</v>
+        <v>382902.8531974667</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>191132.0666898339</v>
+        <v>353231.4143888069</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>328091.1509576063</v>
+        <v>477629.2945913452</v>
       </c>
     </row>
     <row r="10">
@@ -751,37 +751,37 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-1910000</v>
+        <v>-1550000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-1545608.856088561</v>
+        <v>-876568.2656826569</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>-1209454.66428834</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>-899349.321299207</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>-613274.281641335</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>-349367.4184883165</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>-105910.9026644988</v>
+        <v>-255321.2783050342</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>317784.7986115919</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>846480.4415236086</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>1334207.049376023</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>1784139.344442825</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>118679.9790917907</v>
+        <v>2199206.037308879</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>325867.1393835705</v>
+        <v>2582108.890506345</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>516999.2060734044</v>
+        <v>2935340.304895152</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>845090.3570310108</v>
+        <v>3412969.599486498</v>
       </c>
     </row>
     <row r="11">
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>845090.3570310108</v>
+        <v>3412969.599486498</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Added functionality for CVS saving and created a utils file where  most functions have been placed to improve code readability
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,21 @@
       <c r="L1" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="M1" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -534,34 +549,49 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>30000</v>
+        <v>20000</v>
+      </c>
+      <c r="M3" s="7" t="n">
+        <v>20000</v>
+      </c>
+      <c r="N3" s="7" t="n">
+        <v>20000</v>
+      </c>
+      <c r="O3" s="7" t="n">
+        <v>20000</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>20000</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>20000</v>
       </c>
     </row>
     <row r="4">
@@ -571,34 +601,49 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>1400000</v>
+        <v>1050000</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <v>1050000</v>
+      </c>
+      <c r="N4" s="7" t="n">
+        <v>1050000</v>
+      </c>
+      <c r="O4" s="7" t="n">
+        <v>1050000</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>1050000</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <v>1050000</v>
       </c>
     </row>
     <row r="5">
@@ -608,37 +653,52 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-350000</v>
+        <v>-70000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>-700000</v>
+        <v>-350000</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>-350000</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <v>-350000</v>
+      </c>
+      <c r="O5" s="6" t="n">
+        <v>-350000</v>
+      </c>
+      <c r="P5" s="6" t="n">
+        <v>-350000</v>
+      </c>
+      <c r="Q5" s="6" t="n">
+        <v>-350000</v>
       </c>
     </row>
     <row r="6">
@@ -647,8 +707,8 @@
           <t>Residual</t>
         </is>
       </c>
-      <c r="L6" s="7" t="n">
-        <v>140000</v>
+      <c r="Q6" s="7" t="n">
+        <v>70000</v>
       </c>
     </row>
     <row r="7">
@@ -660,7 +720,7 @@
       <c r="B7" s="6" t="n">
         <v>-200000</v>
       </c>
-      <c r="L7" s="7" t="n">
+      <c r="Q7" s="7" t="n">
         <v>200000</v>
       </c>
     </row>
@@ -671,37 +731,52 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-1550000</v>
+        <v>-1270000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="H8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>730000</v>
+        <v>720000</v>
       </c>
       <c r="L8" s="9" t="n">
-        <v>1070000</v>
+        <v>720000</v>
+      </c>
+      <c r="M8" s="9" t="n">
+        <v>720000</v>
+      </c>
+      <c r="N8" s="9" t="n">
+        <v>720000</v>
+      </c>
+      <c r="O8" s="9" t="n">
+        <v>720000</v>
+      </c>
+      <c r="P8" s="9" t="n">
+        <v>720000</v>
+      </c>
+      <c r="Q8" s="9" t="n">
+        <v>990000</v>
       </c>
     </row>
     <row r="9">
@@ -711,37 +786,52 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-1550000</v>
+        <v>-1270000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>673431.7343173431</v>
+        <v>664206.6420664206</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>621246.9873776227</v>
+        <v>612736.7546738198</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>573106.0769166261</v>
+        <v>565255.308739686</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>528695.6429120167</v>
+        <v>521453.2368447288</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>487726.6078524138</v>
+        <v>481045.4214434767</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>449932.2950668024</v>
+        <v>443768.8389699969</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>415066.6928660539</v>
+        <v>409380.8477582997</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>382902.8531974667</v>
+        <v>377657.6086331178</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>353231.4143888069</v>
+        <v>348392.62789033</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>477629.2945913452</v>
+        <v>321395.4131829613</v>
+      </c>
+      <c r="M9" s="7" t="n">
+        <v>296490.2335636174</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>273514.9756121932</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>252320.0882031302</v>
+      </c>
+      <c r="P9" s="7" t="n">
+        <v>232767.609043478</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <v>295254.116637253</v>
       </c>
     </row>
     <row r="10">
@@ -751,37 +841,52 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-1550000</v>
+        <v>-1270000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-876568.2656826569</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <v>-255321.2783050342</v>
+        <v>-605793.3579335794</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>6943.396740240394</v>
       </c>
       <c r="E10" s="7" t="n">
-        <v>317784.7986115919</v>
+        <v>572198.7054799264</v>
       </c>
       <c r="F10" s="7" t="n">
-        <v>846480.4415236086</v>
+        <v>1093651.942324655</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>1334207.049376023</v>
+        <v>1574697.363768132</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>1784139.344442825</v>
+        <v>2018466.202738129</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>2199206.037308879</v>
+        <v>2427847.050496429</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>2582108.890506345</v>
+        <v>2805504.659129546</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>2935340.304895152</v>
+        <v>3153897.287019877</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>3412969.599486498</v>
+        <v>3475292.700202838</v>
+      </c>
+      <c r="M10" s="7" t="n">
+        <v>3771782.933766455</v>
+      </c>
+      <c r="N10" s="7" t="n">
+        <v>4045297.909378649</v>
+      </c>
+      <c r="O10" s="7" t="n">
+        <v>4297617.997581779</v>
+      </c>
+      <c r="P10" s="7" t="n">
+        <v>4530385.606625257</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <v>4825639.72326251</v>
       </c>
     </row>
     <row r="11">
@@ -791,7 +896,7 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>3412969.599486498</v>
+        <v>4825639.72326251</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Database files functionality established
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,21 +516,6 @@
       <c r="L1" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="O1" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="P1" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="3" t="n">
-        <v>15</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -549,49 +534,34 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="M3" s="7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="N3" s="7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="O3" s="7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="Q3" s="7" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4">
@@ -601,49 +571,34 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>1050000</v>
-      </c>
-      <c r="M4" s="7" t="n">
-        <v>1050000</v>
-      </c>
-      <c r="N4" s="7" t="n">
-        <v>1050000</v>
-      </c>
-      <c r="O4" s="7" t="n">
-        <v>1050000</v>
-      </c>
-      <c r="P4" s="7" t="n">
-        <v>1050000</v>
-      </c>
-      <c r="Q4" s="7" t="n">
-        <v>1050000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +608,7 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-70000</v>
+        <v>-140000</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>-350000</v>
@@ -683,21 +638,6 @@
         <v>-350000</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>-350000</v>
-      </c>
-      <c r="M5" s="6" t="n">
-        <v>-350000</v>
-      </c>
-      <c r="N5" s="6" t="n">
-        <v>-350000</v>
-      </c>
-      <c r="O5" s="6" t="n">
-        <v>-350000</v>
-      </c>
-      <c r="P5" s="6" t="n">
-        <v>-350000</v>
-      </c>
-      <c r="Q5" s="6" t="n">
         <v>-350000</v>
       </c>
     </row>
@@ -707,8 +647,8 @@
           <t>Residual</t>
         </is>
       </c>
-      <c r="Q6" s="7" t="n">
-        <v>70000</v>
+      <c r="L6" s="7" t="n">
+        <v>140000</v>
       </c>
     </row>
     <row r="7">
@@ -718,10 +658,10 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>-200000</v>
-      </c>
-      <c r="Q7" s="7" t="n">
-        <v>200000</v>
+        <v>-300000</v>
+      </c>
+      <c r="L7" s="7" t="n">
+        <v>300000</v>
       </c>
     </row>
     <row r="8">
@@ -731,52 +671,37 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-1270000</v>
+        <v>-1440000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="H8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>720000</v>
+        <v>380000</v>
       </c>
       <c r="L8" s="9" t="n">
-        <v>720000</v>
-      </c>
-      <c r="M8" s="9" t="n">
-        <v>720000</v>
-      </c>
-      <c r="N8" s="9" t="n">
-        <v>720000</v>
-      </c>
-      <c r="O8" s="9" t="n">
-        <v>720000</v>
-      </c>
-      <c r="P8" s="9" t="n">
-        <v>720000</v>
-      </c>
-      <c r="Q8" s="9" t="n">
-        <v>990000</v>
+        <v>820000</v>
       </c>
     </row>
     <row r="9">
@@ -786,52 +711,37 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-1270000</v>
+        <v>-1440000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>664206.6420664206</v>
+        <v>350553.5055350553</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>612736.7546738198</v>
+        <v>323388.842744516</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>565255.308739686</v>
+        <v>298329.1907237232</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>521453.2368447288</v>
+        <v>275211.4305569402</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>481045.4214434767</v>
+        <v>253885.0835396127</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>443768.8389699969</v>
+        <v>234211.3316786095</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>409380.8477582997</v>
+        <v>216062.1140946582</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>377657.6086331178</v>
+        <v>199319.2934452566</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>348392.62789033</v>
+        <v>183873.8869421186</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>321395.4131829613</v>
-      </c>
-      <c r="M9" s="7" t="n">
-        <v>296490.2335636174</v>
-      </c>
-      <c r="N9" s="7" t="n">
-        <v>273514.9756121932</v>
-      </c>
-      <c r="O9" s="7" t="n">
-        <v>252320.0882031302</v>
-      </c>
-      <c r="P9" s="7" t="n">
-        <v>232767.609043478</v>
-      </c>
-      <c r="Q9" s="7" t="n">
-        <v>295254.116637253</v>
+        <v>366033.6650139281</v>
       </c>
     </row>
     <row r="10">
@@ -841,52 +751,37 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-1270000</v>
+        <v>-1440000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-605793.3579335794</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>6943.396740240394</v>
-      </c>
-      <c r="E10" s="7" t="n">
-        <v>572198.7054799264</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <v>1093651.942324655</v>
+        <v>-1089446.494464945</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>-766057.6517204286</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>-467728.4609967054</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>-192517.0304397652</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>1574697.363768132</v>
+        <v>61368.05309984752</v>
       </c>
       <c r="H10" s="7" t="n">
-        <v>2018466.202738129</v>
+        <v>295579.384778457</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>2427847.050496429</v>
+        <v>511641.4988731152</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>2805504.659129546</v>
+        <v>710960.7923183718</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>3153897.287019877</v>
+        <v>894834.6792604905</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>3475292.700202838</v>
-      </c>
-      <c r="M10" s="7" t="n">
-        <v>3771782.933766455</v>
-      </c>
-      <c r="N10" s="7" t="n">
-        <v>4045297.909378649</v>
-      </c>
-      <c r="O10" s="7" t="n">
-        <v>4297617.997581779</v>
-      </c>
-      <c r="P10" s="7" t="n">
-        <v>4530385.606625257</v>
-      </c>
-      <c r="Q10" s="7" t="n">
-        <v>4825639.72326251</v>
+        <v>1260868.344274419</v>
       </c>
     </row>
     <row r="11">
@@ -896,7 +791,7 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>4825639.72326251</v>
+        <v>1260868.344274419</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Added image database and updated portofolio to show diagram in portfolio
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +480,7 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>Project lifetime</t>
         </is>
       </c>
       <c r="B1" s="3" t="n">
@@ -501,6 +501,21 @@
       <c r="G1" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="H1" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -519,19 +534,34 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>120000</v>
+        <v>60000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>120000</v>
+        <v>60000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>120000</v>
+        <v>60000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>120000</v>
+        <v>60000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>120000</v>
+        <v>60000</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>60000</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>60000</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>60000</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <v>60000</v>
+      </c>
+      <c r="L3" s="7" t="n">
+        <v>60000</v>
       </c>
     </row>
     <row r="4">
@@ -541,19 +571,34 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>1050000</v>
+        <v>350000</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>1050000</v>
+        <v>350000</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>1050000</v>
+        <v>350000</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>1050000</v>
+        <v>350000</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>1050000</v>
+        <v>350000</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>350000</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>350000</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>350000</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>350000</v>
+      </c>
+      <c r="L4" s="7" t="n">
+        <v>350000</v>
       </c>
     </row>
     <row r="5">
@@ -563,22 +608,37 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-140000</v>
+        <v>-280000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>-350000</v>
+        <v>-140000</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>-140000</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>-140000</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>-140000</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>-140000</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>-140000</v>
       </c>
     </row>
     <row r="6">
@@ -587,7 +647,7 @@
           <t>Residual</t>
         </is>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="L6" s="7" t="n">
         <v>70000</v>
       </c>
     </row>
@@ -600,7 +660,7 @@
       <c r="B7" s="6" t="n">
         <v>-200000</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="L7" s="7" t="n">
         <v>200000</v>
       </c>
     </row>
@@ -611,22 +671,37 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-2340000</v>
+        <v>-2480000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>820000</v>
+        <v>270000</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>820000</v>
+        <v>270000</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>820000</v>
+        <v>270000</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>820000</v>
+        <v>270000</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>1090000</v>
+        <v>270000</v>
+      </c>
+      <c r="H8" s="9" t="n">
+        <v>270000</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>270000</v>
+      </c>
+      <c r="J8" s="9" t="n">
+        <v>270000</v>
+      </c>
+      <c r="K8" s="9" t="n">
+        <v>270000</v>
+      </c>
+      <c r="L8" s="9" t="n">
+        <v>540000</v>
       </c>
     </row>
     <row r="9">
@@ -636,22 +711,37 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-2340000</v>
+        <v>-2480000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>756457.5645756457</v>
+        <v>249077.4907749077</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>697839.0817118502</v>
+        <v>229776.2830026824</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>643762.9905090869</v>
+        <v>211970.7407773822</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>593877.2975176078</v>
+        <v>195544.9638167733</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>728249.3185741522</v>
+        <v>180392.0330413037</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>166413.3146137488</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>153517.8179093624</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>141621.6032374192</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <v>130647.2354588738</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>241046.559887221</v>
       </c>
     </row>
     <row r="10">
@@ -661,22 +751,37 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-2340000</v>
+        <v>-2480000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-1583542.435424354</v>
+        <v>-2230922.509225092</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>-885703.3537125041</v>
+        <v>-2001146.22622241</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>-241940.3632034173</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <v>351936.9343141905</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <v>1080186.252888343</v>
+        <v>-1789175.485445028</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>-1593630.521628254</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>-1413238.488586951</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>-1246825.173973202</v>
+      </c>
+      <c r="I10" s="6" t="n">
+        <v>-1093307.35606384</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>-951685.7528264204</v>
+      </c>
+      <c r="K10" s="6" t="n">
+        <v>-821038.5173675466</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>-579991.9574803256</v>
       </c>
     </row>
     <row r="11">
@@ -685,8 +790,8 @@
           <t>Net Present Value</t>
         </is>
       </c>
-      <c r="B11" s="9" t="n">
-        <v>1080186.252888343</v>
+      <c r="B11" s="8" t="n">
+        <v>-579991.9574803256</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Added sign up Modal feature
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>-2000000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="3">
@@ -534,34 +534,34 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>60000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="4">
@@ -571,34 +571,34 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>350000</v>
+        <v>700000</v>
       </c>
     </row>
     <row r="5">
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-280000</v>
+        <v>-70000</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>-140000</v>
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="L6" s="7" t="n">
-        <v>70000</v>
+        <v>140000</v>
       </c>
     </row>
     <row r="7">
@@ -658,10 +658,10 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>-200000</v>
+        <v>-300000</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>200000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="8">
@@ -671,37 +671,37 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-2480000</v>
+        <v>-1870000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="H8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>270000</v>
+        <v>605000</v>
       </c>
       <c r="L8" s="9" t="n">
-        <v>540000</v>
+        <v>1045000</v>
       </c>
     </row>
     <row r="9">
@@ -711,37 +711,37 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-2480000</v>
+        <v>-1870000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>249077.4907749077</v>
+        <v>558118.0811808117</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>229776.2830026824</v>
+        <v>514869.0785800847</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>211970.7407773822</v>
+        <v>474971.4747048751</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>195544.9638167733</v>
+        <v>438165.5670709179</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>180392.0330413037</v>
+        <v>404211.7777406992</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>166413.3146137488</v>
+        <v>372889.0938567335</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>153517.8179093624</v>
+        <v>343993.6290191268</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>141621.6032374192</v>
+        <v>317337.296143106</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>130647.2354588738</v>
+        <v>292746.5831578468</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>241046.559887221</v>
+        <v>466469.7316336035</v>
       </c>
     </row>
     <row r="10">
@@ -751,37 +751,37 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-2480000</v>
+        <v>-1870000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-2230922.509225092</v>
+        <v>-1311881.918819188</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>-2001146.22622241</v>
+        <v>-797012.8402391034</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>-1789175.485445028</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>-1593630.521628254</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>-1413238.488586951</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>-1246825.173973202</v>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>-1093307.35606384</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>-951685.7528264204</v>
-      </c>
-      <c r="K10" s="6" t="n">
-        <v>-821038.5173675466</v>
-      </c>
-      <c r="L10" s="6" t="n">
-        <v>-579991.9574803256</v>
+        <v>-322041.3655342283</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>116124.2015366896</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>520335.9792773888</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>893225.0731341223</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1237218.702153249</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>1554555.998296355</v>
+      </c>
+      <c r="K10" s="7" t="n">
+        <v>1847302.581454202</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>2313772.313087805</v>
       </c>
     </row>
     <row r="11">
@@ -790,8 +790,8 @@
           <t>Net Present Value</t>
         </is>
       </c>
-      <c r="B11" s="8" t="n">
-        <v>-579991.9574803256</v>
+      <c r="B11" s="9" t="n">
+        <v>2313772.313087805</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Overhaul on core functionalites and integrated sign in / log in functions
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -75,7 +75,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -95,6 +95,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -521,7 +524,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>-500000</v>
+        <v>-2000000</v>
       </c>
     </row>
     <row r="3">
@@ -531,34 +534,34 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="4">
@@ -605,37 +608,37 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-350000</v>
+        <v>-70000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>-2100000</v>
+        <v>-70000</v>
       </c>
     </row>
     <row r="6">
@@ -655,10 +658,10 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>-200000</v>
+        <v>-100000</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>200000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="8">
@@ -668,37 +671,37 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-1050000</v>
-      </c>
-      <c r="C8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="D8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="E8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="F8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="G8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="I8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="J8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="K8" s="8" t="n">
-        <v>-1385000</v>
-      </c>
-      <c r="L8" s="8" t="n">
-        <v>-1115000</v>
+        <v>-2170000</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="G8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="H8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="J8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="K8" s="9" t="n">
+        <v>690000</v>
+      </c>
+      <c r="L8" s="9" t="n">
+        <v>860000</v>
       </c>
     </row>
     <row r="9">
@@ -708,37 +711,37 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-1050000</v>
-      </c>
-      <c r="C9" s="6" t="n">
-        <v>-1277675.276752767</v>
-      </c>
-      <c r="D9" s="6" t="n">
-        <v>-1178667.229476723</v>
-      </c>
-      <c r="E9" s="6" t="n">
-        <v>-1087331.392506202</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>-1003073.240319374</v>
-      </c>
-      <c r="G9" s="6" t="n">
-        <v>-925344.3176377988</v>
-      </c>
-      <c r="H9" s="6" t="n">
-        <v>-853638.6694075635</v>
-      </c>
-      <c r="I9" s="6" t="n">
-        <v>-787489.5474239516</v>
-      </c>
-      <c r="J9" s="6" t="n">
-        <v>-726466.3721623169</v>
-      </c>
-      <c r="K9" s="6" t="n">
-        <v>-670171.9300390377</v>
-      </c>
-      <c r="L9" s="6" t="n">
-        <v>-497716.5079152804</v>
+        <v>-2170000</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>636531.3653136531</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>587206.0565624106</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>541703.0042088658</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>499726.0186428651</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>461001.8622166652</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>425278.4706795804</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>392323.3124350372</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>361921.8749400713</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <v>333876.2683948996</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>383888.9657463148</v>
       </c>
     </row>
     <row r="10">
@@ -748,37 +751,37 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-1050000</v>
+        <v>-2170000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-2327675.276752767</v>
+        <v>-1533468.634686347</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>-3506342.50622949</v>
+        <v>-946262.5781239363</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>-4593673.898735692</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>-5596747.139055066</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>-6522091.456692865</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>-7375730.126100428</v>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>-8163219.67352438</v>
-      </c>
-      <c r="J10" s="6" t="n">
-        <v>-8889686.045686696</v>
-      </c>
-      <c r="K10" s="6" t="n">
-        <v>-9559857.975725733</v>
-      </c>
-      <c r="L10" s="6" t="n">
-        <v>-10057574.48364101</v>
+        <v>-404559.5739150705</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>95166.44472779462</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>556168.3069444598</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>981446.7776240401</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1373770.090059077</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>1735691.964999149</v>
+      </c>
+      <c r="K10" s="7" t="n">
+        <v>2069568.233394048</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>2453457.199140363</v>
       </c>
     </row>
     <row r="11">
@@ -787,8 +790,8 @@
           <t>Net Present Value</t>
         </is>
       </c>
-      <c r="B11" s="8" t="n">
-        <v>-10057574.48364101</v>
+      <c r="B11" s="9" t="n">
+        <v>2453457.199140363</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Major overhaul of the  interaction with databases and web design integration
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>-2000000</v>
+        <v>-2500000</v>
       </c>
     </row>
     <row r="3">
@@ -534,34 +534,34 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>60000</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="4">
@@ -571,34 +571,34 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>700000</v>
+        <v>1400000</v>
       </c>
     </row>
     <row r="5">
@@ -608,37 +608,37 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-70000</v>
+        <v>-1050000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>-70000</v>
+        <v>-700000</v>
       </c>
     </row>
     <row r="6">
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="L6" s="7" t="n">
-        <v>70000</v>
+        <v>140000</v>
       </c>
     </row>
     <row r="7">
@@ -658,10 +658,10 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>-100000</v>
+        <v>-200000</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>100000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="8">
@@ -671,37 +671,37 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-2170000</v>
+        <v>-3750000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="H8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>690000</v>
+        <v>775000</v>
       </c>
       <c r="L8" s="9" t="n">
-        <v>860000</v>
+        <v>1115000</v>
       </c>
     </row>
     <row r="9">
@@ -711,37 +711,37 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-2170000</v>
+        <v>-3750000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>636531.3653136531</v>
+        <v>714944.6494464944</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>587206.0565624106</v>
+        <v>659543.0345447365</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>541703.0042088658</v>
+        <v>608434.5337128565</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>499726.0186428651</v>
+        <v>561286.4702148122</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>461001.8622166652</v>
+        <v>517791.9466926312</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>425278.4706795804</v>
+        <v>477667.8475024272</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>392323.3124350372</v>
+        <v>440652.9958509476</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>361921.8749400713</v>
+        <v>406506.4537370366</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>333876.2683948996</v>
+        <v>375005.9536319525</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>383888.9657463148</v>
+        <v>497716.5079152804</v>
       </c>
     </row>
     <row r="10">
@@ -751,37 +751,37 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-2170000</v>
+        <v>-3750000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-1533468.634686347</v>
+        <v>-3035055.350553506</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>-946262.5781239363</v>
+        <v>-2375512.316008769</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>-404559.5739150705</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <v>95166.44472779462</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <v>556168.3069444598</v>
-      </c>
-      <c r="H10" s="7" t="n">
-        <v>981446.7776240401</v>
+        <v>-1767077.782295913</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>-1205791.3120811</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>-687999.3653884693</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>-210331.5178860421</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>1373770.090059077</v>
+        <v>230321.4779649056</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>1735691.964999149</v>
+        <v>636827.9317019421</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>2069568.233394048</v>
+        <v>1011833.885333895</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>2453457.199140363</v>
+        <v>1509550.393249175</v>
       </c>
     </row>
     <row r="11">
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>2453457.199140363</v>
+        <v>1509550.393249175</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>

<commit_message>
Updating sign in error message functionality
</commit_message>
<xml_diff>
--- a/InvestmentCalc.xlsx
+++ b/InvestmentCalc.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,21 @@
       <c r="L1" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="M1" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -524,7 +539,7 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>-2500000</v>
+        <v>-1500000</v>
       </c>
     </row>
     <row r="3">
@@ -534,34 +549,49 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="H3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="I3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="J3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>75000</v>
+        <v>30000</v>
+      </c>
+      <c r="M3" s="7" t="n">
+        <v>30000</v>
+      </c>
+      <c r="N3" s="7" t="n">
+        <v>30000</v>
+      </c>
+      <c r="O3" s="7" t="n">
+        <v>30000</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>30000</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="4">
@@ -571,34 +601,49 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>1400000</v>
+        <v>910000</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <v>910000</v>
+      </c>
+      <c r="N4" s="7" t="n">
+        <v>910000</v>
+      </c>
+      <c r="O4" s="7" t="n">
+        <v>910000</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>910000</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <v>910000</v>
       </c>
     </row>
     <row r="5">
@@ -608,37 +653,52 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>-1050000</v>
+        <v>-140000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="G5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>-700000</v>
+        <v>-210000</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>-210000</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <v>-210000</v>
+      </c>
+      <c r="O5" s="6" t="n">
+        <v>-210000</v>
+      </c>
+      <c r="P5" s="6" t="n">
+        <v>-210000</v>
+      </c>
+      <c r="Q5" s="6" t="n">
+        <v>-210000</v>
       </c>
     </row>
     <row r="6">
@@ -647,7 +707,7 @@
           <t>Residual</t>
         </is>
       </c>
-      <c r="L6" s="7" t="n">
+      <c r="Q6" s="7" t="n">
         <v>140000</v>
       </c>
     </row>
@@ -658,10 +718,10 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>-200000</v>
-      </c>
-      <c r="L7" s="7" t="n">
-        <v>200000</v>
+        <v>-100000</v>
+      </c>
+      <c r="Q7" s="7" t="n">
+        <v>100000</v>
       </c>
     </row>
     <row r="8">
@@ -671,37 +731,52 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
-        <v>-3750000</v>
+        <v>-1740000</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="G8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="H8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="J8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>775000</v>
+        <v>730000</v>
       </c>
       <c r="L8" s="9" t="n">
-        <v>1115000</v>
+        <v>730000</v>
+      </c>
+      <c r="M8" s="9" t="n">
+        <v>730000</v>
+      </c>
+      <c r="N8" s="9" t="n">
+        <v>730000</v>
+      </c>
+      <c r="O8" s="9" t="n">
+        <v>730000</v>
+      </c>
+      <c r="P8" s="9" t="n">
+        <v>730000</v>
+      </c>
+      <c r="Q8" s="9" t="n">
+        <v>970000</v>
       </c>
     </row>
     <row r="9">
@@ -711,37 +786,52 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>-3750000</v>
+        <v>-1740000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>714944.6494464944</v>
+        <v>673431.7343173431</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>659543.0345447365</v>
+        <v>621246.9873776227</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>608434.5337128565</v>
+        <v>573106.0769166261</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>561286.4702148122</v>
+        <v>528695.6429120167</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>517791.9466926312</v>
+        <v>487726.6078524138</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>477667.8475024272</v>
+        <v>449932.2950668024</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>440652.9958509476</v>
+        <v>415066.6928660539</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>406506.4537370366</v>
+        <v>382902.8531974667</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>375005.9536319525</v>
+        <v>353231.4143888069</v>
       </c>
       <c r="L9" s="7" t="n">
-        <v>497716.5079152804</v>
+        <v>325859.238366058</v>
+      </c>
+      <c r="M9" s="7" t="n">
+        <v>300608.1534742232</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>277313.7947179181</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>255824.5338726181</v>
+      </c>
+      <c r="P9" s="7" t="n">
+        <v>236000.4925024152</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <v>289289.3870082176</v>
       </c>
     </row>
     <row r="10">
@@ -751,37 +841,52 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>-3750000</v>
+        <v>-1740000</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>-3035055.350553506</v>
+        <v>-1066568.265682657</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>-2375512.316008769</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>-1767077.782295913</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>-1205791.3120811</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>-687999.3653884693</v>
-      </c>
-      <c r="H10" s="6" t="n">
-        <v>-210331.5178860421</v>
+        <v>-445321.278305034</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>127784.798611592</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>656480.4415236088</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>1144207.049376023</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>1594139.344442825</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>230321.4779649056</v>
+        <v>2009206.037308879</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>636827.9317019421</v>
+        <v>2392108.890506345</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>1011833.885333895</v>
+        <v>2745340.304895152</v>
       </c>
       <c r="L10" s="7" t="n">
-        <v>1509550.393249175</v>
+        <v>3071199.54326121</v>
+      </c>
+      <c r="M10" s="7" t="n">
+        <v>3371807.696735434</v>
+      </c>
+      <c r="N10" s="7" t="n">
+        <v>3649121.491453352</v>
+      </c>
+      <c r="O10" s="7" t="n">
+        <v>3904946.02532597</v>
+      </c>
+      <c r="P10" s="7" t="n">
+        <v>4140946.517828385</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <v>4430235.904836603</v>
       </c>
     </row>
     <row r="11">
@@ -791,7 +896,7 @@
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>1509550.393249175</v>
+        <v>4430235.904836603</v>
       </c>
     </row>
     <row r="12"/>

</xml_diff>